<commit_message>
Revisione e parte meta euristica
</commit_message>
<xml_diff>
--- a/statistics/data.xlsx
+++ b/statistics/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="7575" tabRatio="748" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="7575" tabRatio="940" firstSheet="6" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Random cplex" sheetId="1" r:id="rId1"/>
@@ -1155,355 +1155,6 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="it-IT"/>
-              <a:t>Confronto dei</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="it-IT" baseline="0"/>
-              <a:t> tempi di risoluzione con distribuzione random</a:t>
-            </a:r>
-            <a:endParaRPr lang="it-IT"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="1"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>Media tempi distribuzione random con risolutore CPlex</c:v>
-          </c:tx>
-          <c:cat>
-            <c:numRef>
-              <c:f>Statistics!$A$3:$A$14</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>100</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Statistics!$C$22:$C$33</c:f>
-              <c:numCache>
-                <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* \-??_-;_-@_-</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>9519.48</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>17052.579999999998</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>16602.36</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>21157.060000000005</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>32084.52</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>35338.9</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>38044.060000000005</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>42797.760000000002</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>54998.54</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>70692.180000000008</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>63203.199999999997</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>66344.260000000009</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-497F-44D9-85FC-C97653CB6FD8}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>Media tempi distribuzione random con metaeuristica</c:v>
-          </c:tx>
-          <c:cat>
-            <c:numRef>
-              <c:f>Statistics!$A$3:$A$14</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>100</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Statistics!$C$3:$C$14</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>18.8</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>73.400000000000006</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>238</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>396.6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1871.6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6053.6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>13307.6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>20883</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>40550.400000000001</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>92110.8</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>256190.6</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>506618.8</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-497F-44D9-85FC-C97653CB6FD8}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="87597056"/>
-        <c:axId val="87598976"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="87597056"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="it-IT"/>
-                  <a:t>ID Serie</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87598976"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="87598976"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" vert="horz"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="it-IT"/>
-                  <a:t>Tempo medio (ms)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="_-* #,##0_-;\-* #,##0_-;_-* \-??_-;_-@_-" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87597056"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="it-IT"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
               <a:rPr lang="it-IT" baseline="0"/>
               <a:t>confronto tra classi con CPlex</a:t>
             </a:r>
@@ -1945,7 +1596,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="it-IT"/>
@@ -2398,7 +2049,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="it-IT"/>
@@ -2890,7 +2541,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="it-IT"/>
@@ -3359,7 +3010,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="it-IT"/>
@@ -3714,7 +3365,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="it-IT"/>
@@ -4064,7 +3715,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="it-IT"/>
@@ -4489,7 +4140,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="88" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="88" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4497,47 +4148,6 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>304800</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Grafico 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
@@ -4570,7 +4180,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
@@ -4597,7 +4207,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
@@ -4611,6 +4221,33 @@
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9308523" cy="6093835"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Grafico 1"/>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks noGrp="1"/>
         </xdr:cNvGraphicFramePr>
@@ -4685,33 +4322,6 @@
 </file>
 
 <file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:absoluteAnchor>
-    <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9308523" cy="6093835"/>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Grafico 1"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks noGrp="1"/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:absoluteAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
@@ -35023,7 +34633,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
+    <sheetView topLeftCell="N1" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
       <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
@@ -35895,6 +35505,5 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>